<commit_message>
Update .gitignore & totals
</commit_message>
<xml_diff>
--- a/Hardware/orders/totals.xlsx
+++ b/Hardware/orders/totals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xia_t\Desktop\Projects\riscv\rv32i_dev\Hardware\orders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA222E43-E6DC-44D5-85E8-142D9267358E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B435B0-29C8-495B-8769-DEFA112C8416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9390" yWindow="2550" windowWidth="15105" windowHeight="13050" xr2:uid="{B7C40B04-CF42-4CBF-9AFF-82D8975A26D6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B7C40B04-CF42-4CBF-9AFF-82D8975A26D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Price (cad)</t>
   </si>
@@ -87,13 +87,16 @@
   </si>
   <si>
     <t>5.pdf</t>
+  </si>
+  <si>
+    <t>Discount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +106,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -193,22 +205,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -230,6 +233,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,7 +560,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,115 +577,119 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="16" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>20.68</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="18"/>
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="5">
         <v>19.239999999999998</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="18"/>
+      <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="5">
         <v>25.18</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="14" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="18"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="6">
+        <v>-11.41</v>
+      </c>
+      <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="8">
         <v>60.99</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="10" t="s">
+      <c r="A7" s="18"/>
+      <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="7">
         <v>8</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="18"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="15"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C10">
         <f>SUM(C2:C8)</f>
-        <v>134.09</v>
+        <v>122.68</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C11">
         <f>C10/10</f>
-        <v>13.409000000000001</v>
+        <v>12.268000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="11">
         <f>C10/2</f>
-        <v>67.045000000000002</v>
+        <v>61.34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>